<commit_message>
Finish data cleaning and wrangling
</commit_message>
<xml_diff>
--- a/Data/Dicionário de dados por arquivo.xlsx
+++ b/Data/Dicionário de dados por arquivo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcd2753435410c94/Learning/EMAp/Data Science/Homeworks/Homework2/Homework2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valte\OneDrive\Learning\EMAp\Data Science\Homeworks\Homework2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C02D016-2AB0-439A-9C82-405F1172D70C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{4C02D016-2AB0-439A-9C82-405F1172D70C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E0554BE6-AE3A-4036-B38A-1E5D0F3F3EA6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Escolares" sheetId="2" r:id="rId1"/>
@@ -2802,7 +2802,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2817,12 +2817,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2899,6 +2893,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8F5C55AA-D2F5-4751-9AD6-D284EF5B22FD}" name="Tabela4" displayName="Tabela4" ref="A1:B249" totalsRowShown="0">
   <autoFilter ref="A1:B249" xr:uid="{C0B2CD1E-B991-4F7D-BB97-E16FF795EDAC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B249">
+    <sortCondition ref="A1:A249"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C4F10156-32F1-4924-A0E4-8E5AF9BE0E4A}" name="CAMPO"/>
     <tableColumn id="2" xr3:uid="{00CCC37B-27B7-4BCD-82BF-F8B747A39382}" name="DESCRIÇÃO"/>
@@ -2921,6 +2918,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF54344E-D4B3-4242-B05D-5FEDF378D6BA}" name="Tabela1" displayName="Tabela1" ref="A1:B136" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B136" xr:uid="{A672EB23-3C19-4E6E-B957-0F3F8ECAC957}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B136">
+    <sortCondition ref="A1:A136"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E8C315DC-9E3D-4D57-A714-6D168F006610}" name="CAMPO"/>
     <tableColumn id="2" xr3:uid="{E0D0D6B8-F108-48A0-A94A-A615E9688264}" name="DESCRIÇÃO"/>
@@ -3260,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3280,1986 +3280,1986 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>262</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>269</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>360</v>
+        <v>325</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>361</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>362</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>359</v>
+        <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
-        <v>363</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>367</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>368</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>369</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>370</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>371</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>372</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>373</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B44" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>272</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="B47" t="s">
-        <v>273</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>274</v>
+        <v>347</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>286</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="B56" t="s">
-        <v>287</v>
+        <v>352</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>350</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>289</v>
+        <v>353</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>290</v>
+        <v>351</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B60" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>292</v>
+        <v>337</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>293</v>
+        <v>339</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B67" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B76" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B82" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B84" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B85" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="B86" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B87" t="s">
-        <v>318</v>
+        <v>289</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B88" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B89" t="s">
-        <v>320</v>
+        <v>291</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="B90" t="s">
-        <v>321</v>
+        <v>292</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B91" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B92" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B93" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B95" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="B97" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="B98" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="B99" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="B103" t="s">
-        <v>334</v>
+        <v>248</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>335</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>336</v>
+        <v>252</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>262</v>
       </c>
       <c r="B106" t="s">
-        <v>337</v>
+        <v>263</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>259</v>
       </c>
       <c r="B107" t="s">
-        <v>338</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="B108" t="s">
-        <v>339</v>
+        <v>267</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>340</v>
+        <v>266</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="B110" t="s">
-        <v>341</v>
+        <v>475</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>191</v>
       </c>
       <c r="B111" t="s">
-        <v>356</v>
+        <v>416</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="B112" t="s">
-        <v>357</v>
+        <v>455</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="B113" t="s">
-        <v>342</v>
+        <v>404</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B114" t="s">
-        <v>343</v>
+        <v>386</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>229</v>
       </c>
       <c r="B115" t="s">
-        <v>344</v>
+        <v>434</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="B116" t="s">
-        <v>345</v>
+        <v>465</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="B117" t="s">
-        <v>346</v>
+        <v>407</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>113</v>
+        <v>200</v>
       </c>
       <c r="B118" t="s">
-        <v>347</v>
+        <v>445</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="B119" t="s">
-        <v>348</v>
+        <v>395</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B120" t="s">
-        <v>349</v>
+        <v>390</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>218</v>
       </c>
       <c r="B121" t="s">
-        <v>350</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="B122" t="s">
-        <v>351</v>
+        <v>474</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="B123" t="s">
-        <v>352</v>
+        <v>415</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="B124" t="s">
-        <v>353</v>
+        <v>454</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="B125" t="s">
-        <v>354</v>
+        <v>403</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B126" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>228</v>
       </c>
       <c r="B127" t="s">
-        <v>376</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B128" t="s">
-        <v>377</v>
+        <v>466</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="B129" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
       <c r="B130" t="s">
-        <v>378</v>
+        <v>446</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="B131" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>219</v>
       </c>
       <c r="B133" t="s">
-        <v>381</v>
+        <v>426</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B134" t="s">
-        <v>438</v>
+        <v>463</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="B135" t="s">
-        <v>382</v>
+        <v>467</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>198</v>
       </c>
       <c r="B136" t="s">
-        <v>383</v>
+        <v>443</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="B137" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B138" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>217</v>
       </c>
       <c r="B139" t="s">
-        <v>386</v>
+        <v>423</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="B140" t="s">
-        <v>387</v>
+        <v>461</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="B141" t="s">
-        <v>388</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="B142" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="B143" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B144" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
       <c r="B145" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>141</v>
+        <v>237</v>
       </c>
       <c r="B146" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="B148" t="s">
-        <v>465</v>
+        <v>412</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
       <c r="B149" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="B150" t="s">
-        <v>467</v>
+        <v>400</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B151" t="s">
-        <v>468</v>
+        <v>382</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="B152" t="s">
-        <v>469</v>
+        <v>430</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="B153" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>149</v>
+        <v>242</v>
       </c>
       <c r="B154" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B155" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="B156" t="s">
-        <v>473</v>
+        <v>410</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
       <c r="B157" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B158" t="s">
-        <v>475</v>
+        <v>398</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B159" t="s">
-        <v>476</v>
+        <v>380</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
       <c r="B160" t="s">
-        <v>391</v>
+        <v>422</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>156</v>
+        <v>239</v>
       </c>
       <c r="B161" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B162" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="B163" t="s">
-        <v>392</v>
+        <v>468</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="B164" t="s">
-        <v>393</v>
+        <v>444</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B165" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B166" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="B167" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>163</v>
+        <v>240</v>
       </c>
       <c r="B168" t="s">
-        <v>396</v>
+        <v>474</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B169" t="s">
-        <v>397</v>
+        <v>469</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="B170" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="B171" t="s">
-        <v>399</v>
+        <v>449</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B172" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="B173" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="B174" t="s">
-        <v>401</v>
+        <v>429</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B175" t="s">
-        <v>402</v>
+        <v>472</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B176" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>172</v>
+        <v>207</v>
       </c>
       <c r="B177" t="s">
-        <v>404</v>
+        <v>452</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B178" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="B179" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="B180" t="s">
-        <v>463</v>
+        <v>431</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B181" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="B182" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="B183" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B184" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="B185" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="B186" t="s">
-        <v>407</v>
+        <v>470</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="B187" t="s">
-        <v>408</v>
+        <v>472</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="B188" t="s">
-        <v>409</v>
+        <v>476</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B189" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="B190" t="s">
-        <v>411</v>
+        <v>456</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B191" t="s">
-        <v>440</v>
+        <v>405</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="B192" t="s">
-        <v>412</v>
+        <v>387</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="B193" t="s">
-        <v>413</v>
+        <v>435</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="B194" t="s">
-        <v>414</v>
+        <v>473</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B195" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="B196" t="s">
-        <v>416</v>
+        <v>453</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="B197" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>132</v>
       </c>
       <c r="B198" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>194</v>
+        <v>227</v>
       </c>
       <c r="B199" t="s">
-        <v>465</v>
+        <v>432</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B200" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B201" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B202" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="B203" t="s">
-        <v>443</v>
+        <v>397</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="B204" t="s">
-        <v>444</v>
+        <v>379</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="B205" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>201</v>
+        <v>155</v>
       </c>
       <c r="B206" t="s">
-        <v>446</v>
+        <v>391</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B207" t="s">
-        <v>447</v>
+        <v>418</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B208" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="B209" t="s">
-        <v>449</v>
+        <v>406</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>205</v>
+        <v>136</v>
       </c>
       <c r="B210" t="s">
-        <v>450</v>
+        <v>388</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="B211" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>207</v>
+        <v>148</v>
       </c>
       <c r="B212" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="B213" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B214" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="B215" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>211</v>
+        <v>129</v>
       </c>
       <c r="B216" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B217" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>213</v>
+        <v>140</v>
       </c>
       <c r="B218" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="B219" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="B220" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>216</v>
+        <v>159</v>
       </c>
       <c r="B221" t="s">
-        <v>424</v>
+        <v>393</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>217</v>
+        <v>121</v>
       </c>
       <c r="B222" t="s">
-        <v>423</v>
+        <v>375</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B223" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>219</v>
+        <v>6</v>
       </c>
       <c r="B224" t="s">
-        <v>426</v>
+        <v>374</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>220</v>
+        <v>24</v>
       </c>
       <c r="B225" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>221</v>
+        <v>9</v>
       </c>
       <c r="B226" t="s">
-        <v>428</v>
+        <v>257</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>222</v>
+        <v>4</v>
       </c>
       <c r="B227" t="s">
-        <v>422</v>
+        <v>251</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>223</v>
+        <v>8</v>
       </c>
       <c r="B228" t="s">
-        <v>429</v>
+        <v>256</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
       <c r="B229" t="s">
-        <v>441</v>
+        <v>255</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>225</v>
+        <v>10</v>
       </c>
       <c r="B230" t="s">
-        <v>430</v>
+        <v>258</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="B231" t="s">
-        <v>431</v>
+        <v>254</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>227</v>
+        <v>11</v>
       </c>
       <c r="B232" t="s">
-        <v>432</v>
+        <v>261</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>228</v>
+        <v>14</v>
       </c>
       <c r="B233" t="s">
-        <v>433</v>
+        <v>265</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>229</v>
+        <v>16</v>
       </c>
       <c r="B234" t="s">
-        <v>434</v>
+        <v>265</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>230</v>
+        <v>106</v>
       </c>
       <c r="B235" t="s">
-        <v>435</v>
+        <v>356</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B236" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>232</v>
+        <v>107</v>
       </c>
       <c r="B237" t="s">
-        <v>469</v>
+        <v>357</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>233</v>
+        <v>3</v>
       </c>
       <c r="B238" t="s">
-        <v>470</v>
+        <v>250</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B239" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>235</v>
+        <v>158</v>
       </c>
       <c r="B240" t="s">
-        <v>420</v>
+        <v>392</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="B241" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="B242" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>238</v>
+        <v>177</v>
       </c>
       <c r="B243" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>239</v>
+        <v>139</v>
       </c>
       <c r="B244" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B245" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>475</v>
+        <v>355</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>242</v>
+        <v>35</v>
       </c>
       <c r="B247" t="s">
-        <v>476</v>
+        <v>373</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>243</v>
+        <v>114</v>
       </c>
       <c r="B248" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>244</v>
+        <v>12</v>
       </c>
       <c r="B249" t="s">
-        <v>355</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5276,7 +5276,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB54AD1-690A-466E-8D49-9941CC6396E0}">
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -6058,8 +6060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9B9610-2764-41C2-B771-7263DA7139E8}">
   <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6078,706 +6080,706 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>648</v>
+        <v>746</v>
       </c>
       <c r="B2" t="s">
-        <v>649</v>
+        <v>747</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>650</v>
+        <v>754</v>
       </c>
       <c r="B3" t="s">
-        <v>651</v>
+        <v>755</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>652</v>
+        <v>762</v>
       </c>
       <c r="B4" t="s">
-        <v>653</v>
+        <v>763</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>654</v>
+        <v>770</v>
       </c>
       <c r="B5" t="s">
-        <v>655</v>
+        <v>771</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>656</v>
+        <v>778</v>
       </c>
       <c r="B6" t="s">
-        <v>657</v>
+        <v>779</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>658</v>
+        <v>786</v>
       </c>
       <c r="B7" t="s">
-        <v>659</v>
+        <v>787</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>660</v>
+        <v>794</v>
       </c>
       <c r="B8" t="s">
-        <v>661</v>
+        <v>795</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>662</v>
+        <v>802</v>
       </c>
       <c r="B9" t="s">
-        <v>663</v>
+        <v>803</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>664</v>
+        <v>744</v>
       </c>
       <c r="B10" t="s">
-        <v>665</v>
+        <v>745</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>666</v>
+        <v>752</v>
       </c>
       <c r="B11" t="s">
-        <v>667</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>668</v>
+        <v>760</v>
       </c>
       <c r="B12" t="s">
-        <v>669</v>
+        <v>761</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>916</v>
+      <c r="A13" t="s">
+        <v>768</v>
+      </c>
+      <c r="B13" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>671</v>
+        <v>784</v>
       </c>
       <c r="B14" t="s">
-        <v>672</v>
+        <v>785</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>673</v>
+        <v>792</v>
       </c>
       <c r="B15" t="s">
-        <v>674</v>
+        <v>793</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>675</v>
+        <v>800</v>
       </c>
       <c r="B16" t="s">
-        <v>676</v>
+        <v>801</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>677</v>
+        <v>740</v>
       </c>
       <c r="B17" t="s">
-        <v>678</v>
+        <v>741</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>679</v>
+        <v>748</v>
       </c>
       <c r="B18" t="s">
-        <v>680</v>
+        <v>749</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>681</v>
+        <v>756</v>
       </c>
       <c r="B19" t="s">
-        <v>681</v>
+        <v>757</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>682</v>
+        <v>764</v>
       </c>
       <c r="B20" t="s">
-        <v>683</v>
+        <v>765</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>684</v>
+        <v>772</v>
       </c>
       <c r="B21" t="s">
-        <v>685</v>
+        <v>773</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>686</v>
+        <v>780</v>
       </c>
       <c r="B22" t="s">
-        <v>687</v>
+        <v>781</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>688</v>
+        <v>788</v>
       </c>
       <c r="B23" t="s">
-        <v>689</v>
+        <v>789</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>690</v>
+        <v>796</v>
       </c>
       <c r="B24" t="s">
-        <v>691</v>
+        <v>797</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>692</v>
+        <v>742</v>
       </c>
       <c r="B25" t="s">
-        <v>693</v>
+        <v>743</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>694</v>
+        <v>750</v>
       </c>
       <c r="B26" t="s">
-        <v>695</v>
+        <v>751</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>696</v>
+        <v>758</v>
       </c>
       <c r="B27" t="s">
-        <v>697</v>
+        <v>759</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>698</v>
+        <v>766</v>
       </c>
       <c r="B28" t="s">
-        <v>699</v>
+        <v>767</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>700</v>
+        <v>774</v>
       </c>
       <c r="B29" t="s">
-        <v>701</v>
+        <v>775</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>702</v>
+        <v>782</v>
       </c>
       <c r="B30" t="s">
-        <v>703</v>
+        <v>783</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>704</v>
+        <v>790</v>
       </c>
       <c r="B31" t="s">
-        <v>705</v>
+        <v>791</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>706</v>
+        <v>798</v>
       </c>
       <c r="B32" t="s">
-        <v>707</v>
+        <v>799</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>708</v>
+        <v>776</v>
       </c>
       <c r="B33" t="s">
-        <v>709</v>
+        <v>777</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>710</v>
+        <v>673</v>
       </c>
       <c r="B34" t="s">
-        <v>711</v>
+        <v>674</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>712</v>
+        <v>690</v>
       </c>
       <c r="B35" t="s">
-        <v>713</v>
+        <v>691</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>714</v>
+        <v>675</v>
       </c>
       <c r="B36" t="s">
-        <v>715</v>
+        <v>676</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>716</v>
+        <v>906</v>
       </c>
       <c r="B37" t="s">
-        <v>717</v>
+        <v>907</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>718</v>
+        <v>908</v>
       </c>
       <c r="B38" t="s">
-        <v>719</v>
+        <v>909</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>720</v>
-      </c>
-      <c r="B39" t="s">
-        <v>721</v>
+      <c r="A39" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>722</v>
+        <v>668</v>
       </c>
       <c r="B40" t="s">
-        <v>723</v>
+        <v>669</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>724</v>
+        <v>666</v>
       </c>
       <c r="B41" t="s">
-        <v>725</v>
+        <v>667</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>726</v>
+        <v>654</v>
       </c>
       <c r="B42" t="s">
-        <v>727</v>
+        <v>655</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>728</v>
+        <v>656</v>
       </c>
       <c r="B43" t="s">
-        <v>729</v>
+        <v>657</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>730</v>
+        <v>662</v>
       </c>
       <c r="B44" t="s">
-        <v>731</v>
+        <v>663</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>732</v>
+        <v>681</v>
       </c>
       <c r="B45" t="s">
-        <v>733</v>
+        <v>681</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>734</v>
+        <v>804</v>
       </c>
       <c r="B46" t="s">
-        <v>735</v>
+        <v>805</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>736</v>
+        <v>806</v>
       </c>
       <c r="B47" t="s">
-        <v>737</v>
+        <v>807</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>738</v>
+        <v>808</v>
       </c>
       <c r="B48" t="s">
-        <v>739</v>
+        <v>809</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>740</v>
+        <v>810</v>
       </c>
       <c r="B49" t="s">
-        <v>741</v>
+        <v>811</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>742</v>
+        <v>812</v>
       </c>
       <c r="B50" t="s">
-        <v>743</v>
+        <v>813</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>744</v>
+        <v>814</v>
       </c>
       <c r="B51" t="s">
-        <v>745</v>
+        <v>815</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>746</v>
+        <v>816</v>
       </c>
       <c r="B52" t="s">
-        <v>747</v>
+        <v>817</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>748</v>
+        <v>818</v>
       </c>
       <c r="B53" t="s">
-        <v>749</v>
+        <v>819</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>750</v>
+        <v>732</v>
       </c>
       <c r="B54" t="s">
-        <v>751</v>
+        <v>733</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>752</v>
+        <v>734</v>
       </c>
       <c r="B55" t="s">
-        <v>753</v>
+        <v>735</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>754</v>
+        <v>736</v>
       </c>
       <c r="B56" t="s">
-        <v>755</v>
+        <v>737</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>756</v>
+        <v>738</v>
       </c>
       <c r="B57" t="s">
-        <v>757</v>
+        <v>739</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>758</v>
+        <v>677</v>
       </c>
       <c r="B58" t="s">
-        <v>759</v>
+        <v>678</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>760</v>
+        <v>910</v>
       </c>
       <c r="B59" t="s">
-        <v>761</v>
+        <v>911</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>762</v>
+        <v>710</v>
       </c>
       <c r="B60" t="s">
-        <v>763</v>
+        <v>711</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>764</v>
+        <v>692</v>
       </c>
       <c r="B61" t="s">
-        <v>765</v>
+        <v>693</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>766</v>
+        <v>728</v>
       </c>
       <c r="B62" t="s">
-        <v>767</v>
+        <v>729</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>768</v>
+        <v>730</v>
       </c>
       <c r="B63" t="s">
-        <v>769</v>
+        <v>731</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>770</v>
+        <v>716</v>
       </c>
       <c r="B64" t="s">
-        <v>771</v>
+        <v>717</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>772</v>
+        <v>718</v>
       </c>
       <c r="B65" t="s">
-        <v>773</v>
+        <v>719</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>774</v>
+        <v>712</v>
       </c>
       <c r="B66" t="s">
-        <v>775</v>
+        <v>713</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>776</v>
+        <v>714</v>
       </c>
       <c r="B67" t="s">
-        <v>777</v>
+        <v>715</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>778</v>
+        <v>720</v>
       </c>
       <c r="B68" t="s">
-        <v>779</v>
+        <v>721</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>780</v>
+        <v>722</v>
       </c>
       <c r="B69" t="s">
-        <v>781</v>
+        <v>723</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>782</v>
+        <v>724</v>
       </c>
       <c r="B70" t="s">
-        <v>783</v>
+        <v>725</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>784</v>
+        <v>726</v>
       </c>
       <c r="B71" t="s">
-        <v>785</v>
+        <v>727</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>786</v>
+        <v>648</v>
       </c>
       <c r="B72" t="s">
-        <v>787</v>
+        <v>649</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>788</v>
+        <v>890</v>
       </c>
       <c r="B73" t="s">
-        <v>789</v>
+        <v>891</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>790</v>
+        <v>850</v>
       </c>
       <c r="B74" t="s">
-        <v>791</v>
+        <v>851</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>792</v>
+        <v>892</v>
       </c>
       <c r="B75" t="s">
-        <v>793</v>
+        <v>893</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>794</v>
+        <v>852</v>
       </c>
       <c r="B76" t="s">
-        <v>795</v>
+        <v>853</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>796</v>
+        <v>894</v>
       </c>
       <c r="B77" t="s">
-        <v>797</v>
+        <v>895</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>798</v>
+        <v>854</v>
       </c>
       <c r="B78" t="s">
-        <v>799</v>
+        <v>855</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>800</v>
+        <v>896</v>
       </c>
       <c r="B79" t="s">
-        <v>801</v>
+        <v>897</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>802</v>
+        <v>856</v>
       </c>
       <c r="B80" t="s">
-        <v>803</v>
+        <v>857</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>804</v>
+        <v>898</v>
       </c>
       <c r="B81" t="s">
-        <v>805</v>
+        <v>899</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>806</v>
+        <v>858</v>
       </c>
       <c r="B82" t="s">
-        <v>807</v>
+        <v>859</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>808</v>
+        <v>912</v>
       </c>
       <c r="B83" t="s">
-        <v>809</v>
+        <v>913</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>810</v>
+        <v>914</v>
       </c>
       <c r="B84" t="s">
-        <v>811</v>
+        <v>915</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>812</v>
+        <v>684</v>
       </c>
       <c r="B85" t="s">
-        <v>813</v>
+        <v>685</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>814</v>
+        <v>652</v>
       </c>
       <c r="B86" t="s">
-        <v>815</v>
+        <v>653</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>816</v>
+        <v>902</v>
       </c>
       <c r="B87" t="s">
-        <v>817</v>
+        <v>903</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>818</v>
+        <v>650</v>
       </c>
       <c r="B88" t="s">
-        <v>819</v>
+        <v>651</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>820</v>
+        <v>862</v>
       </c>
       <c r="B89" t="s">
-        <v>821</v>
+        <v>863</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -6790,210 +6792,210 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>824</v>
+        <v>868</v>
       </c>
       <c r="B91" t="s">
-        <v>825</v>
+        <v>869</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B92" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>828</v>
+        <v>874</v>
       </c>
       <c r="B93" t="s">
-        <v>829</v>
+        <v>875</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="B94" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>832</v>
+        <v>880</v>
       </c>
       <c r="B95" t="s">
-        <v>833</v>
+        <v>881</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>834</v>
+        <v>840</v>
       </c>
       <c r="B96" t="s">
-        <v>835</v>
+        <v>841</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>836</v>
+        <v>886</v>
       </c>
       <c r="B97" t="s">
-        <v>837</v>
+        <v>887</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>838</v>
+        <v>846</v>
       </c>
       <c r="B98" t="s">
-        <v>839</v>
+        <v>847</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>840</v>
+        <v>904</v>
       </c>
       <c r="B99" t="s">
-        <v>841</v>
+        <v>905</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>842</v>
+        <v>860</v>
       </c>
       <c r="B100" t="s">
-        <v>843</v>
+        <v>861</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>844</v>
+        <v>820</v>
       </c>
       <c r="B101" t="s">
-        <v>845</v>
+        <v>821</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>846</v>
+        <v>866</v>
       </c>
       <c r="B102" t="s">
-        <v>847</v>
+        <v>867</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>848</v>
+        <v>826</v>
       </c>
       <c r="B103" t="s">
-        <v>849</v>
+        <v>827</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>850</v>
+        <v>872</v>
       </c>
       <c r="B104" t="s">
-        <v>851</v>
+        <v>873</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>852</v>
+        <v>832</v>
       </c>
       <c r="B105" t="s">
-        <v>853</v>
+        <v>833</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>854</v>
+        <v>878</v>
       </c>
       <c r="B106" t="s">
-        <v>855</v>
+        <v>879</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>856</v>
+        <v>838</v>
       </c>
       <c r="B107" t="s">
-        <v>857</v>
+        <v>839</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>858</v>
+        <v>884</v>
       </c>
       <c r="B108" t="s">
-        <v>859</v>
+        <v>885</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>860</v>
+        <v>844</v>
       </c>
       <c r="B109" t="s">
-        <v>861</v>
+        <v>845</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>862</v>
+        <v>664</v>
       </c>
       <c r="B110" t="s">
-        <v>863</v>
+        <v>665</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>864</v>
+        <v>658</v>
       </c>
       <c r="B111" t="s">
-        <v>865</v>
+        <v>659</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>866</v>
+        <v>660</v>
       </c>
       <c r="B112" t="s">
-        <v>867</v>
+        <v>661</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="B113" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>870</v>
+        <v>824</v>
       </c>
       <c r="B114" t="s">
-        <v>871</v>
+        <v>825</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B115" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>874</v>
+        <v>830</v>
       </c>
       <c r="B116" t="s">
-        <v>875</v>
+        <v>831</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -7006,154 +7008,154 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>878</v>
+        <v>836</v>
       </c>
       <c r="B118" t="s">
-        <v>879</v>
+        <v>837</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B119" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>882</v>
+        <v>842</v>
       </c>
       <c r="B120" t="s">
-        <v>883</v>
+        <v>843</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="B121" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>886</v>
+        <v>848</v>
       </c>
       <c r="B122" t="s">
-        <v>887</v>
+        <v>849</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>888</v>
+        <v>679</v>
       </c>
       <c r="B123" t="s">
-        <v>889</v>
+        <v>680</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>890</v>
+        <v>686</v>
       </c>
       <c r="B124" t="s">
-        <v>891</v>
+        <v>687</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>892</v>
+        <v>688</v>
       </c>
       <c r="B125" t="s">
-        <v>893</v>
+        <v>689</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>894</v>
+        <v>900</v>
       </c>
       <c r="B126" t="s">
-        <v>895</v>
+        <v>901</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>896</v>
+        <v>698</v>
       </c>
       <c r="B127" t="s">
-        <v>897</v>
+        <v>699</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>898</v>
+        <v>700</v>
       </c>
       <c r="B128" t="s">
-        <v>899</v>
+        <v>701</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>900</v>
+        <v>694</v>
       </c>
       <c r="B129" t="s">
-        <v>901</v>
+        <v>695</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>902</v>
+        <v>696</v>
       </c>
       <c r="B130" t="s">
-        <v>903</v>
+        <v>697</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>904</v>
+        <v>702</v>
       </c>
       <c r="B131" t="s">
-        <v>905</v>
+        <v>703</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>906</v>
+        <v>704</v>
       </c>
       <c r="B132" t="s">
-        <v>907</v>
+        <v>705</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>908</v>
+        <v>706</v>
       </c>
       <c r="B133" t="s">
-        <v>909</v>
+        <v>707</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>910</v>
+        <v>708</v>
       </c>
       <c r="B134" t="s">
-        <v>911</v>
+        <v>709</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>912</v>
+        <v>682</v>
       </c>
       <c r="B135" t="s">
-        <v>913</v>
+        <v>683</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>914</v>
+        <v>671</v>
       </c>
       <c r="B136" t="s">
-        <v>915</v>
+        <v>672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>